<commit_message>
Updates to architecture presentation, committed uncommitted stuff
</commit_message>
<xml_diff>
--- a/Agendas/201905 Montreal WGM FHIR Agenda.xlsx
+++ b/Agendas/201905 Montreal WGM FHIR Agenda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Documents\SVN\FHIR-documents\Agendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35635BBF-C2BC-49CD-945F-C1F37BFE599A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB28EBD-C7F5-4C97-91FB-9ACA6593E3D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7860" yWindow="0" windowWidth="9495" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
   <si>
     <t>Mon</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>Public Health</t>
+  </si>
+  <si>
+    <t>MGC</t>
+  </si>
+  <si>
+    <t>Grahame</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Lloyd Tue lunch Peter Bomberg</t>
   </si>
 </sst>
 </file>
@@ -275,18 +287,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -295,10 +307,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -640,13 +655,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +671,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
@@ -669,8 +684,14 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,7 +708,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -707,7 +728,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -724,7 +745,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -741,7 +762,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
@@ -758,7 +779,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +791,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -787,7 +808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -804,7 +825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -821,7 +842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -838,7 +859,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -846,14 +867,11 @@
         <v>41</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
@@ -870,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
@@ -888,7 +906,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -900,7 +918,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -917,7 +935,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
@@ -933,11 +951,11 @@
       <c r="F17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -955,22 +973,27 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
@@ -987,7 +1010,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
@@ -996,194 +1019,192 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="C29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="3" t="s">
+      <c r="C31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>52</v>
@@ -1198,9 +1219,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>52</v>
@@ -1215,68 +1236,85 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="1">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="1">
         <v>8</v>
       </c>
     </row>

</xml_diff>